<commit_message>
Tidy format table with tsv (txt due to excel)
</commit_message>
<xml_diff>
--- a/Data/Survey_Data.xlsx
+++ b/Data/Survey_Data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trvrb/Documents/src/tfcb_2019/homeworks/homework01/messy-project-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\OneDrive\Documents\MCB Courses\MCB 536 TFCB\tfcb-homework01\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A2EF31-99BB-1147-875E-0BF67F65B824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F562BF9F-A7BB-4BAB-A127-D2ED8639A0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1400" windowWidth="25120" windowHeight="15580" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="481" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
     <sheet name="2014" sheetId="2" r:id="rId2"/>
+    <sheet name="Tidy" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="44">
   <si>
     <t>NA</t>
   </si>
@@ -140,6 +141,27 @@
   </si>
   <si>
     <t>gray cell means my measurement device wasn't calibrated correctly</t>
+  </si>
+  <si>
+    <t>Calibrated Scale</t>
+  </si>
+  <si>
+    <t>Field Season</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>OL</t>
   </si>
 </sst>
 </file>
@@ -149,7 +171,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -162,11 +184,13 @@
     <font>
       <sz val="18"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="28"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
@@ -177,16 +201,29 @@
       <b/>
       <sz val="24"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
       <color rgb="FF808080"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -317,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -334,12 +371,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,7 +776,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -775,7 +820,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -803,27 +848,27 @@
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="24.75" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="1"/>
-    <col min="3" max="3" width="26.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.1328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.46484375" style="1"/>
+    <col min="3" max="3" width="26.1328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.46484375" customWidth="1"/>
+    <col min="5" max="5" width="12.796875" customWidth="1"/>
+    <col min="6" max="6" width="14.796875" style="2" customWidth="1"/>
     <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.46484375" style="1" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="24.83203125" customWidth="1"/>
-    <col min="16" max="16" width="52.83203125" customWidth="1"/>
+    <col min="13" max="13" width="24.796875" customWidth="1"/>
+    <col min="16" max="16" width="52.796875" customWidth="1"/>
     <col min="17" max="17" width="18" customWidth="1"/>
-    <col min="20" max="20" width="11.5" style="1"/>
-    <col min="21" max="21" width="19.83203125" customWidth="1"/>
-    <col min="26" max="26" width="17.5" customWidth="1"/>
-    <col min="29" max="16384" width="11.5" style="1"/>
+    <col min="20" max="20" width="11.46484375" style="1"/>
+    <col min="21" max="21" width="19.796875" customWidth="1"/>
+    <col min="26" max="26" width="17.46484375" customWidth="1"/>
+    <col min="29" max="16384" width="11.46484375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:17" ht="79" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:17" ht="79.05" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C3" s="11" t="s">
         <v>20</v>
       </c>
@@ -842,7 +887,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -859,7 +904,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -876,7 +921,7 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
@@ -899,298 +944,298 @@
       <c r="P6" s="14"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="17" t="s">
+      <c r="P7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C8" s="18">
+    <row r="8" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
+      <c r="C8" s="17">
         <v>41471</v>
       </c>
-      <c r="D8" s="16">
-        <v>2</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="17"/>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="16"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="18">
+      <c r="H8" s="17">
         <v>41505</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="5">
         <v>8</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="17">
+      <c r="J8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="16">
         <v>52</v>
       </c>
       <c r="L8" s="5"/>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <v>41590</v>
       </c>
-      <c r="N8" s="16">
+      <c r="N8" s="5">
         <v>9</v>
       </c>
-      <c r="O8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P8" s="17">
+      <c r="O8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="16">
         <v>117</v>
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C9" s="18">
+    <row r="9" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
+      <c r="C9" s="17">
         <v>41471</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="5">
         <v>7</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="E9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="18">
+      <c r="H9" s="17">
         <v>41564</v>
       </c>
-      <c r="I9" s="16">
-        <v>3</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="17">
+      <c r="I9" s="5">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="16">
         <v>33</v>
       </c>
       <c r="L9" s="5"/>
-      <c r="M9" s="18">
+      <c r="M9" s="17">
         <v>41591</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="5">
         <v>11</v>
       </c>
-      <c r="O9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P9" s="17">
+      <c r="O9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="16">
         <v>126</v>
       </c>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C10" s="18">
+    <row r="10" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
+      <c r="C10" s="17">
         <v>41471</v>
       </c>
-      <c r="D10" s="16">
-        <v>3</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="17"/>
+      <c r="D10" s="5">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="18">
+      <c r="H10" s="17">
         <v>41564</v>
       </c>
-      <c r="I10" s="16">
-        <v>3</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="17">
+      <c r="I10" s="5">
+        <v>3</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="16">
         <v>50</v>
       </c>
       <c r="L10" s="5"/>
-      <c r="M10" s="18">
+      <c r="M10" s="17">
         <v>41591</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="5">
         <v>17</v>
       </c>
-      <c r="O10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="P10" s="17" t="s">
+      <c r="O10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P10" s="16" t="s">
         <v>27</v>
       </c>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C11" s="18">
+    <row r="11" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
+      <c r="C11" s="17">
         <v>41471</v>
       </c>
-      <c r="D11" s="16">
-        <v>1</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="17"/>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="16"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <v>41618</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="5">
         <v>9</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="17">
+      <c r="J11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="16">
         <v>40</v>
       </c>
       <c r="L11" s="5"/>
-      <c r="M11" s="18">
+      <c r="M11" s="17">
         <v>41591</v>
       </c>
-      <c r="N11" s="16">
+      <c r="N11" s="5">
         <v>14</v>
       </c>
-      <c r="O11" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="17" t="s">
+      <c r="O11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="16" t="s">
         <v>28</v>
       </c>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C12" s="18">
+    <row r="12" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
+      <c r="C12" s="17">
         <v>41473</v>
       </c>
-      <c r="D12" s="16">
-        <v>3</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="17" t="s">
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="18">
+      <c r="H12" s="17">
         <v>41618</v>
       </c>
-      <c r="I12" s="16">
-        <v>1</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="17">
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="16">
         <v>45</v>
       </c>
       <c r="L12" s="5"/>
-      <c r="M12" s="18">
+      <c r="M12" s="17">
         <v>41591</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="5">
         <v>11</v>
       </c>
-      <c r="O12" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P12" s="17">
+      <c r="O12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="16">
         <v>122</v>
       </c>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C13" s="18">
+    <row r="13" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
+      <c r="C13" s="17">
         <v>41473</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="5">
         <v>7</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="17" t="s">
+      <c r="E13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="19">
+      <c r="H13" s="18">
         <v>41619</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="19">
         <v>8</v>
       </c>
-      <c r="J13" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="21">
+      <c r="J13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="20">
         <v>41</v>
       </c>
       <c r="L13" s="5"/>
-      <c r="M13" s="18">
+      <c r="M13" s="17">
         <v>41591</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N13" s="5">
         <v>4</v>
       </c>
-      <c r="O13" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P13" s="17">
+      <c r="O13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" s="16">
         <v>107</v>
       </c>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C14" s="18">
+    <row r="14" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
+      <c r="C14" s="17">
         <v>41473</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="5">
         <v>4</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="17" t="s">
+      <c r="E14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="5"/>
@@ -1199,31 +1244,31 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="19">
+      <c r="M14" s="18">
         <v>41591</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="19">
         <v>4</v>
       </c>
-      <c r="O14" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="P14" s="21">
+      <c r="O14" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" s="20">
         <v>115</v>
       </c>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C15" s="19">
+    <row r="15" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
+      <c r="C15" s="18">
         <v>41473</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="19">
         <v>6</v>
       </c>
-      <c r="E15" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="21" t="s">
+      <c r="E15" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>26</v>
       </c>
       <c r="G15" s="5"/>
@@ -1238,7 +1283,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1255,7 +1300,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1272,7 +1317,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1289,7 +1334,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1306,7 +1351,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1323,7 +1368,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1340,7 +1385,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1357,7 +1402,7 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="G23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
@@ -1366,7 +1411,7 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="G24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
@@ -1375,22 +1420,22 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="G25" s="5"/>
       <c r="L25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="G26" s="5"/>
       <c r="L26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="G27" s="5"/>
       <c r="L27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="G28" s="5"/>
       <c r="L28" s="5"/>
       <c r="Q28" s="5"/>
@@ -1410,29 +1455,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="24.75" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="1" customWidth="1"/>
-    <col min="5" max="7" width="11.5" style="1"/>
-    <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" style="1" customWidth="1"/>
-    <col min="10" max="12" width="11.5" style="1"/>
-    <col min="13" max="13" width="22.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.1640625" style="1" customWidth="1"/>
-    <col min="15" max="19" width="11.5" style="1"/>
+    <col min="3" max="3" width="22.46484375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1328125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="11.46484375" style="1"/>
+    <col min="8" max="8" width="22.46484375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1328125" style="1" customWidth="1"/>
+    <col min="10" max="12" width="11.46484375" style="1"/>
+    <col min="13" max="13" width="22.46484375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.1328125" style="1" customWidth="1"/>
+    <col min="15" max="19" width="11.46484375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:17" ht="69" customHeight="1" x14ac:dyDescent="0.95">
       <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
@@ -1455,7 +1500,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1496,7 +1541,7 @@
       </c>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C8" s="6">
         <v>41648</v>
       </c>
@@ -1533,7 +1578,7 @@
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C9" s="6">
         <v>41648</v>
       </c>
@@ -1572,7 +1617,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C10" s="6">
         <v>41711</v>
       </c>
@@ -1607,7 +1652,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C11" s="6">
         <v>41711</v>
       </c>
@@ -1648,7 +1693,7 @@
       </c>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C12" s="6">
         <v>41711</v>
       </c>
@@ -1685,7 +1730,7 @@
       </c>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1718,7 +1763,7 @@
       </c>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1747,7 +1792,7 @@
       </c>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1772,7 +1817,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1797,7 +1842,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1822,7 +1867,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1839,7 +1884,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1856,7 +1901,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1873,7 +1918,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1890,7 +1935,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="3:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:17" ht="30.75" x14ac:dyDescent="0.9">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1909,7 +1954,7 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -1926,7 +1971,7 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1943,7 +1988,7 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -1960,7 +2005,7 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -1977,7 +2022,7 @@
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C27" s="4" t="s">
         <v>29</v>
       </c>
@@ -1996,7 +2041,7 @@
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C28" s="4" t="s">
         <v>16</v>
       </c>
@@ -2019,7 +2064,7 @@
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C29" s="6">
         <v>28498</v>
       </c>
@@ -2042,7 +2087,7 @@
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C30" s="6">
         <v>28498</v>
       </c>
@@ -2063,7 +2108,7 @@
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C31" s="6">
         <v>28498</v>
       </c>
@@ -2086,7 +2131,7 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C32" s="6">
         <v>28498</v>
       </c>
@@ -2109,7 +2154,7 @@
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C33" s="6">
         <v>28498</v>
       </c>
@@ -2132,7 +2177,7 @@
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
     </row>
-    <row r="34" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -2149,7 +2194,7 @@
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
     </row>
-    <row r="35" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -2166,7 +2211,7 @@
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
     </row>
-    <row r="36" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -2183,7 +2228,7 @@
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
     </row>
-    <row r="37" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -2198,7 +2243,7 @@
       <c r="P37" s="5"/>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -2215,7 +2260,7 @@
       <c r="P38" s="5"/>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="L39" s="5"/>
@@ -2225,7 +2270,7 @@
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="L40" s="5"/>
@@ -2235,7 +2280,7 @@
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
     </row>
-    <row r="41" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="L41" s="5"/>
@@ -2245,34 +2290,34 @@
       <c r="P41" s="5"/>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="L42" s="5"/>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="L43" s="5"/>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="G44" s="5"/>
       <c r="L44" s="5"/>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="G45" s="5"/>
       <c r="L45" s="5"/>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="G46" s="5"/>
       <c r="L46" s="5"/>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:17" ht="29.65" x14ac:dyDescent="0.75">
       <c r="G47" s="5"/>
       <c r="L47" s="5"/>
       <c r="Q47" s="5"/>
@@ -2286,4 +2331,1151 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F8B9767-CB8F-4C1E-90AE-ABBDB343F385}">
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A2" s="22">
+        <v>41471</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="23">
+        <v>2</v>
+      </c>
+      <c r="G2" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A3" s="22">
+        <v>41471</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="23">
+        <v>7</v>
+      </c>
+      <c r="G3" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A4" s="22">
+        <v>41471</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="23">
+        <v>3</v>
+      </c>
+      <c r="G4" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A5" s="22">
+        <v>41471</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="23">
+        <v>1</v>
+      </c>
+      <c r="G5" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A6" s="22">
+        <v>41473</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="23">
+        <v>3</v>
+      </c>
+      <c r="G6" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A7" s="22">
+        <v>41473</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="23">
+        <v>7</v>
+      </c>
+      <c r="G7" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A8" s="22">
+        <v>41473</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="23">
+        <v>4</v>
+      </c>
+      <c r="G8" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A9" s="22">
+        <v>41473</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="23">
+        <v>6</v>
+      </c>
+      <c r="G9" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A10" s="22">
+        <v>41505</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="23">
+        <v>52</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="23">
+        <v>8</v>
+      </c>
+      <c r="G10" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A11" s="22">
+        <v>41564</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="23">
+        <v>33</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="23">
+        <v>3</v>
+      </c>
+      <c r="G11" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A12" s="22">
+        <v>41564</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="23">
+        <v>50</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="23">
+        <v>3</v>
+      </c>
+      <c r="G12" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A13" s="22">
+        <v>41618</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="23">
+        <v>40</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="23">
+        <v>9</v>
+      </c>
+      <c r="G13" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A14" s="22">
+        <v>41618</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="23">
+        <v>45</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="23">
+        <v>1</v>
+      </c>
+      <c r="G14" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A15" s="22">
+        <v>41619</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="23">
+        <v>41</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="23">
+        <v>8</v>
+      </c>
+      <c r="G15" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A16" s="22">
+        <v>41590</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="23">
+        <v>117</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="23">
+        <v>9</v>
+      </c>
+      <c r="G16" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A17" s="22">
+        <v>41591</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="23">
+        <v>126</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="23">
+        <v>11</v>
+      </c>
+      <c r="G17" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A18" s="22">
+        <v>41591</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="23">
+        <v>132</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="23">
+        <v>17</v>
+      </c>
+      <c r="G18" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A19" s="22">
+        <v>41591</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="23">
+        <v>113</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="23">
+        <v>14</v>
+      </c>
+      <c r="G19" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A20" s="22">
+        <v>41591</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="23">
+        <v>122</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="23">
+        <v>11</v>
+      </c>
+      <c r="G20" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A21" s="22">
+        <v>41591</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="23">
+        <v>107</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="23">
+        <v>4</v>
+      </c>
+      <c r="G21" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A22" s="22">
+        <v>41591</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="23">
+        <v>115</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="23">
+        <v>4</v>
+      </c>
+      <c r="G22" s="21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A23" s="22">
+        <v>41648</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="23">
+        <v>40</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="23">
+        <v>1</v>
+      </c>
+      <c r="G23" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A24" s="22">
+        <v>41648</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="23">
+        <v>36</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="23">
+        <v>1</v>
+      </c>
+      <c r="G24" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A25" s="22">
+        <v>41711</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="23">
+        <v>51</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="23">
+        <v>1</v>
+      </c>
+      <c r="G25" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A26" s="22">
+        <v>41711</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="23">
+        <v>44</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="23">
+        <v>1</v>
+      </c>
+      <c r="G26" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A27" s="22">
+        <v>41711</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="23">
+        <v>146</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="23">
+        <v>1</v>
+      </c>
+      <c r="G27" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A28" s="22">
+        <v>41647</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="23">
+        <v>2</v>
+      </c>
+      <c r="G28" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A29" s="22">
+        <v>41647</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="23">
+        <v>44</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="23">
+        <v>2</v>
+      </c>
+      <c r="G29" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A30" s="22">
+        <v>41647</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="23">
+        <v>7</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="23">
+        <v>2</v>
+      </c>
+      <c r="G30" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A31" s="22">
+        <v>41647</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="23">
+        <v>45</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="23">
+        <v>2</v>
+      </c>
+      <c r="G31" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A32" s="22">
+        <v>41647</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="23">
+        <v>2</v>
+      </c>
+      <c r="G32" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A33" s="22">
+        <v>41647</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="23">
+        <v>157</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="23">
+        <v>2</v>
+      </c>
+      <c r="G33" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A34" s="22">
+        <v>41647</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="23">
+        <v>2</v>
+      </c>
+      <c r="G34" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A35" s="22">
+        <v>41688</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="23">
+        <v>218</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="23">
+        <v>2</v>
+      </c>
+      <c r="G35" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A36" s="22">
+        <v>41688</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="23">
+        <v>7</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="23">
+        <v>2</v>
+      </c>
+      <c r="G36" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A37" s="22">
+        <v>41688</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="23">
+        <v>52</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="23">
+        <v>2</v>
+      </c>
+      <c r="G37" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A38" s="22">
+        <v>42074</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="23">
+        <v>8</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="23">
+        <v>3</v>
+      </c>
+      <c r="G38" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A39" s="22">
+        <v>42102</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="23">
+        <v>3</v>
+      </c>
+      <c r="G39" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A40" s="22">
+        <v>42130</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="23">
+        <v>3</v>
+      </c>
+      <c r="G40" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A41" s="22">
+        <v>42142</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="23">
+        <v>182</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="23">
+        <v>3</v>
+      </c>
+      <c r="G41" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A42" s="22">
+        <v>42164</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="23">
+        <v>29</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="23">
+        <v>3</v>
+      </c>
+      <c r="G42" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A43" s="22">
+        <v>42193</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="23">
+        <v>115</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="23">
+        <v>3</v>
+      </c>
+      <c r="G43" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A44" s="22">
+        <v>42193</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="23">
+        <v>190</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F44" s="23">
+        <v>3</v>
+      </c>
+      <c r="G44" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A45" s="22">
+        <v>28498</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="23">
+        <v>37</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" s="23">
+        <v>4</v>
+      </c>
+      <c r="G45" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A46" s="22">
+        <v>28498</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46" s="23">
+        <v>4</v>
+      </c>
+      <c r="G46" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A47" s="22">
+        <v>28498</v>
+      </c>
+      <c r="B47" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="23">
+        <v>48</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" s="23">
+        <v>4</v>
+      </c>
+      <c r="G47" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A48" s="22">
+        <v>28498</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="23">
+        <v>52</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="23">
+        <v>4</v>
+      </c>
+      <c r="G48" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A49" s="22">
+        <v>28498</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="23">
+        <v>35</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" s="23">
+        <v>4</v>
+      </c>
+      <c r="G49" s="21">
+        <v>2014</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>